<commit_message>
:recycle: refactor: alterar nome da empresa na ficha para cemag
</commit_message>
<xml_diff>
--- a/FICHA DE EPI.xlsx
+++ b/FICHA DE EPI.xlsx
@@ -81,7 +81,7 @@
     <t>Declaro que:</t>
   </si>
   <si>
-    <t>Pelo presente, declaro ter sido treinado e recebido da Fortel, a título de empréstimo, para meu uso exclusivo e obrigatório nas dependências da empresa, conforme determinado na NR 6 da Portaria 3.214/78, os equipamentos especificados neste termo de responsabilidade, de acordo com a necessidade de meu cargo/função comprometendo-me a mantê-los em perfeito estado de conservação, ficando ciente de que:</t>
+    <t>Pelo presente, declaro ter sido treinado e recebido da Cemag, a título de empréstimo, para meu uso exclusivo e obrigatório nas dependências da empresa, conforme determinado na NR 6 da Portaria 3.214/78, os equipamentos especificados neste termo de responsabilidade, de acordo com a necessidade de meu cargo/função comprometendo-me a mantê-los em perfeito estado de conservação, ficando ciente de que:</t>
   </si>
   <si>
     <t>1. Fico PROIBIDO DE DAR ou EMPRESTAR o equipamento que estiver sob minha responsabilidade, só podendo fazê-lo se receber ordem por escrito da pessoa autorizada para este fim.</t>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -435,7 +435,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -444,6 +444,9 @@
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1191,6 +1194,7 @@
     <row r="12" ht="1.5" customHeight="1">
       <c r="A12" s="24"/>
       <c r="H12" s="25"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" ht="52.5" customHeight="1">
       <c r="A13" s="26"/>
@@ -1206,7 +1210,6 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -1221,7 +1224,7 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="22"/>
@@ -1243,7 +1246,7 @@
       <c r="H15" s="28"/>
     </row>
     <row r="16" ht="24.75" customHeight="1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="22"/>
@@ -1283,7 +1286,7 @@
       <c r="H17" s="28"/>
     </row>
     <row r="18" ht="34.5" customHeight="1">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="22"/>
@@ -1323,7 +1326,7 @@
       <c r="H19" s="28"/>
     </row>
     <row r="20">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="22"/>
@@ -1345,33 +1348,33 @@
       <c r="H21" s="28"/>
     </row>
     <row r="22" ht="77.25" customHeight="1">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="27"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
     </row>
     <row r="23" ht="21.75" customHeight="1">
-      <c r="A23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
+      <c r="A23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="41"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
     </row>
     <row r="24" ht="21.75" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="22"/>
@@ -1387,10 +1390,10 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
@@ -1409,118 +1412,118 @@
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="28"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="43" t="s">
+      <c r="G26" s="44" t="s">
         <v>29</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="J26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="37"/>
+      <c r="J26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
     </row>
     <row r="27" ht="76.5" customHeight="1">
-      <c r="A27" s="44"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="48"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="49"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" ht="17.25" customHeight="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="53"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="54"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="54"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="53"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="54"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="53"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="53"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="54"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="56"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="57"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="54"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="56"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="57"/>
       <c r="H33" s="3"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="O33" s="57"/>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="57"/>
-      <c r="R33" s="57"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
@@ -1531,22 +1534,22 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" ht="16.5" customHeight="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="53"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="3"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="O34" s="57"/>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="57"/>
-      <c r="R34" s="57"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
@@ -1557,22 +1560,22 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" ht="16.5" customHeight="1">
-      <c r="A35" s="58"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="59"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
       <c r="H35" s="3"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="O35" s="57"/>
-      <c r="P35" s="57"/>
-      <c r="Q35" s="57"/>
-      <c r="R35" s="57"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
@@ -1583,22 +1586,22 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36" ht="16.5" customHeight="1">
-      <c r="A36" s="49"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="53"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="3"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
@@ -1609,22 +1612,22 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37" ht="16.5" customHeight="1">
-      <c r="A37" s="54"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="53"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="54"/>
       <c r="H37" s="3"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="O37" s="57"/>
-      <c r="P37" s="57"/>
-      <c r="Q37" s="57"/>
-      <c r="R37" s="57"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
@@ -1635,22 +1638,22 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38" ht="16.5" customHeight="1">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="53"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="54"/>
       <c r="H38" s="3"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
@@ -1661,22 +1664,22 @@
       <c r="Z38" s="4"/>
     </row>
     <row r="39" ht="16.5" customHeight="1">
-      <c r="A39" s="55"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="53"/>
+      <c r="A39" s="56"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="54"/>
       <c r="H39" s="3"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="57"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
@@ -1687,22 +1690,22 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40" ht="16.5" customHeight="1">
-      <c r="A40" s="54"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="53"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="54"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="R40" s="57"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
       <c r="S40" s="4"/>
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
@@ -1713,22 +1716,22 @@
       <c r="Z40" s="4"/>
     </row>
     <row r="41" ht="16.5" customHeight="1">
-      <c r="A41" s="54"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="53"/>
+      <c r="A41" s="55"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="54"/>
       <c r="H41" s="3"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="O41" s="57"/>
-      <c r="P41" s="57"/>
-      <c r="Q41" s="57"/>
-      <c r="R41" s="57"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="58"/>
+      <c r="R41" s="58"/>
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
@@ -1739,22 +1742,22 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42" ht="16.5" customHeight="1">
-      <c r="A42" s="54"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="53"/>
+      <c r="A42" s="55"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="54"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="O42" s="57"/>
-      <c r="P42" s="57"/>
-      <c r="Q42" s="57"/>
-      <c r="R42" s="57"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="58"/>
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
@@ -1765,22 +1768,22 @@
       <c r="Z42" s="4"/>
     </row>
     <row r="43" ht="16.5" customHeight="1">
-      <c r="A43" s="54"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="53"/>
+      <c r="A43" s="55"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="3"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="O43" s="57"/>
-      <c r="P43" s="57"/>
-      <c r="Q43" s="57"/>
-      <c r="R43" s="57"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="58"/>
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
@@ -1791,22 +1794,22 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44" ht="16.5" customHeight="1">
-      <c r="A44" s="54"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="53"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="54"/>
       <c r="H44" s="3"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="58"/>
+      <c r="R44" s="58"/>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
@@ -1817,581 +1820,581 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="60"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="53"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="54"/>
       <c r="H45" s="3"/>
-      <c r="J45" s="65"/>
-      <c r="K45" s="66"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="66"/>
-      <c r="O45" s="35"/>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="37"/>
-      <c r="R45" s="37"/>
+      <c r="J45" s="66"/>
+      <c r="K45" s="67"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="38"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="60"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="53"/>
+      <c r="A46" s="61"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="3"/>
-      <c r="J46" s="65"/>
-      <c r="K46" s="69"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="69"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="70"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="70"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="60"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="70"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="71"/>
       <c r="H47" s="3"/>
-      <c r="J47" s="65"/>
-      <c r="K47" s="66"/>
-      <c r="M47" s="65"/>
-      <c r="N47" s="66"/>
-      <c r="O47" s="71"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="67"/>
+      <c r="M47" s="66"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="72"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="60"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="53"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="3"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="75"/>
-      <c r="M48" s="76"/>
-      <c r="N48" s="77"/>
+      <c r="J48" s="75"/>
+      <c r="K48" s="76"/>
+      <c r="M48" s="77"/>
+      <c r="N48" s="78"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="78"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="70"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="71"/>
       <c r="H49" s="3"/>
-      <c r="J49" s="65"/>
-      <c r="K49" s="66"/>
-      <c r="M49" s="65"/>
-      <c r="N49" s="66"/>
-      <c r="O49" s="71"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="67"/>
+      <c r="M49" s="66"/>
+      <c r="N49" s="67"/>
+      <c r="O49" s="72"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="61"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="53"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="54"/>
       <c r="H50" s="3"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="82"/>
-      <c r="M50" s="71"/>
-      <c r="N50" s="83"/>
+      <c r="J50" s="82"/>
+      <c r="K50" s="83"/>
+      <c r="M50" s="72"/>
+      <c r="N50" s="84"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="60"/>
-      <c r="B51" s="61"/>
-      <c r="C51" s="84"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="53"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="54"/>
       <c r="H51" s="3"/>
-      <c r="J51" s="85"/>
-      <c r="K51" s="75"/>
-      <c r="M51" s="81"/>
-      <c r="N51" s="75"/>
+      <c r="J51" s="86"/>
+      <c r="K51" s="76"/>
+      <c r="M51" s="82"/>
+      <c r="N51" s="76"/>
     </row>
     <row r="52">
-      <c r="A52" s="60"/>
-      <c r="B52" s="61"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="53"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="54"/>
       <c r="H52" s="3"/>
-      <c r="J52" s="81"/>
-      <c r="K52" s="75"/>
-      <c r="M52" s="81"/>
-      <c r="N52" s="86"/>
+      <c r="J52" s="82"/>
+      <c r="K52" s="76"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="87"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="60"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="53"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="54"/>
       <c r="H53" s="3"/>
-      <c r="J53" s="81"/>
-      <c r="K53" s="75"/>
-      <c r="M53" s="65"/>
-      <c r="N53" s="69"/>
+      <c r="J53" s="82"/>
+      <c r="K53" s="76"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="70"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="60"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="53"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="54"/>
       <c r="H54" s="3"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="75"/>
-      <c r="M54" s="81"/>
-      <c r="N54" s="75"/>
+      <c r="J54" s="86"/>
+      <c r="K54" s="76"/>
+      <c r="M54" s="82"/>
+      <c r="N54" s="76"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="60"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="87"/>
-      <c r="E55" s="64"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="53"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="54"/>
       <c r="H55" s="3"/>
-      <c r="J55" s="81"/>
-      <c r="K55" s="86"/>
-      <c r="M55" s="88"/>
-      <c r="N55" s="89"/>
+      <c r="J55" s="82"/>
+      <c r="K55" s="87"/>
+      <c r="M55" s="89"/>
+      <c r="N55" s="90"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="60"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="53"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="54"/>
       <c r="H56" s="3"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="60"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="64"/>
-      <c r="F57" s="64"/>
-      <c r="G57" s="53"/>
+      <c r="A57" s="61"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="54"/>
       <c r="H57" s="3"/>
-      <c r="J57" s="35"/>
-      <c r="M57" s="35"/>
+      <c r="J57" s="36"/>
+      <c r="M57" s="36"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="60"/>
-      <c r="B58" s="61"/>
-      <c r="C58" s="90"/>
-      <c r="D58" s="91"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="53"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="91"/>
+      <c r="D58" s="92"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="54"/>
       <c r="H58" s="3"/>
-      <c r="J58" s="65"/>
-      <c r="K58" s="66"/>
-      <c r="M58" s="65"/>
-      <c r="N58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="67"/>
+      <c r="M58" s="66"/>
+      <c r="N58" s="67"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="60"/>
-      <c r="B59" s="92"/>
-      <c r="C59" s="90"/>
-      <c r="D59" s="91"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="53"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="91"/>
+      <c r="D59" s="92"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="54"/>
       <c r="H59" s="3"/>
-      <c r="J59" s="65"/>
-      <c r="K59" s="66"/>
-      <c r="M59" s="65"/>
-      <c r="N59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="67"/>
+      <c r="M59" s="66"/>
+      <c r="N59" s="67"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="93"/>
-      <c r="B60" s="92"/>
-      <c r="C60" s="94"/>
-      <c r="D60" s="63"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="53"/>
+      <c r="A60" s="94"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="54"/>
       <c r="H60" s="3"/>
-      <c r="J60" s="65"/>
-      <c r="K60" s="66"/>
-      <c r="M60" s="65"/>
-      <c r="N60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="67"/>
+      <c r="M60" s="66"/>
+      <c r="N60" s="67"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="93"/>
-      <c r="B61" s="50"/>
-      <c r="C61" s="95"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="53"/>
+      <c r="A61" s="94"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="96"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="54"/>
       <c r="H61" s="3"/>
-      <c r="J61" s="65"/>
-      <c r="K61" s="69"/>
-      <c r="M61" s="65"/>
-      <c r="N61" s="69"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="70"/>
+      <c r="M61" s="66"/>
+      <c r="N61" s="70"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="93"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="95"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="53"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="96"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="54"/>
       <c r="H62" s="3"/>
-      <c r="J62" s="65"/>
-      <c r="K62" s="69"/>
-      <c r="M62" s="81"/>
-      <c r="N62" s="75"/>
+      <c r="J62" s="66"/>
+      <c r="K62" s="70"/>
+      <c r="M62" s="82"/>
+      <c r="N62" s="76"/>
     </row>
     <row r="63" ht="17.25" customHeight="1">
-      <c r="A63" s="96"/>
-      <c r="J63" s="65"/>
-      <c r="K63" s="69"/>
-      <c r="M63" s="74"/>
-      <c r="N63" s="75"/>
+      <c r="A63" s="97"/>
+      <c r="J63" s="66"/>
+      <c r="K63" s="70"/>
+      <c r="M63" s="75"/>
+      <c r="N63" s="76"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="96"/>
-      <c r="J64" s="71"/>
-      <c r="K64" s="69"/>
-      <c r="M64" s="76"/>
-      <c r="N64" s="77"/>
+      <c r="A64" s="97"/>
+      <c r="J64" s="72"/>
+      <c r="K64" s="70"/>
+      <c r="M64" s="77"/>
+      <c r="N64" s="78"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="96"/>
-      <c r="M65" s="76"/>
-      <c r="N65" s="77"/>
+      <c r="A65" s="97"/>
+      <c r="M65" s="77"/>
+      <c r="N65" s="78"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="96"/>
-      <c r="J66" s="35"/>
-      <c r="M66" s="35"/>
+      <c r="A66" s="97"/>
+      <c r="J66" s="36"/>
+      <c r="M66" s="36"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="96"/>
-      <c r="J67" s="65"/>
-      <c r="K67" s="66"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="66"/>
+      <c r="A67" s="97"/>
+      <c r="J67" s="66"/>
+      <c r="K67" s="67"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="67"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="96"/>
-      <c r="J68" s="65"/>
-      <c r="K68" s="66"/>
-      <c r="M68" s="65"/>
-      <c r="N68" s="66"/>
+      <c r="A68" s="97"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="67"/>
+      <c r="M68" s="66"/>
+      <c r="N68" s="67"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="96"/>
-      <c r="J69" s="65"/>
-      <c r="K69" s="66"/>
-      <c r="M69" s="65"/>
-      <c r="N69" s="66"/>
+      <c r="A69" s="97"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="67"/>
+      <c r="M69" s="66"/>
+      <c r="N69" s="67"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="96"/>
-      <c r="J70" s="65"/>
-      <c r="K70" s="69"/>
-      <c r="M70" s="65"/>
-      <c r="N70" s="69"/>
+      <c r="A70" s="97"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="70"/>
+      <c r="M70" s="66"/>
+      <c r="N70" s="70"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="96"/>
-      <c r="J71" s="74"/>
-      <c r="K71" s="75"/>
-      <c r="M71" s="74"/>
-      <c r="N71" s="75"/>
+      <c r="A71" s="97"/>
+      <c r="J71" s="75"/>
+      <c r="K71" s="76"/>
+      <c r="M71" s="75"/>
+      <c r="N71" s="76"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="96"/>
-      <c r="J72" s="81"/>
-      <c r="K72" s="75"/>
-      <c r="M72" s="81"/>
-      <c r="N72" s="75"/>
+      <c r="A72" s="97"/>
+      <c r="J72" s="82"/>
+      <c r="K72" s="76"/>
+      <c r="M72" s="82"/>
+      <c r="N72" s="76"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="96"/>
-      <c r="J73" s="97"/>
-      <c r="K73" s="98"/>
-      <c r="M73" s="97"/>
-      <c r="N73" s="98"/>
+      <c r="A73" s="97"/>
+      <c r="J73" s="98"/>
+      <c r="K73" s="99"/>
+      <c r="M73" s="98"/>
+      <c r="N73" s="99"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="96"/>
-      <c r="J74" s="97"/>
-      <c r="K74" s="99"/>
-      <c r="M74" s="97"/>
-      <c r="N74" s="99"/>
+      <c r="A74" s="97"/>
+      <c r="J74" s="98"/>
+      <c r="K74" s="100"/>
+      <c r="M74" s="98"/>
+      <c r="N74" s="100"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="96"/>
-      <c r="J75" s="85"/>
-      <c r="K75" s="98"/>
-      <c r="M75" s="85"/>
-      <c r="N75" s="98"/>
+      <c r="A75" s="97"/>
+      <c r="J75" s="86"/>
+      <c r="K75" s="99"/>
+      <c r="M75" s="86"/>
+      <c r="N75" s="99"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="96"/>
+      <c r="A76" s="97"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="96"/>
-      <c r="J77" s="35"/>
+      <c r="A77" s="97"/>
+      <c r="J77" s="36"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="96"/>
-      <c r="J78" s="65"/>
-      <c r="K78" s="66"/>
-      <c r="M78" s="65"/>
-      <c r="N78" s="66"/>
+      <c r="A78" s="97"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="67"/>
+      <c r="M78" s="66"/>
+      <c r="N78" s="67"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="96"/>
-      <c r="J79" s="65"/>
-      <c r="K79" s="66"/>
-      <c r="M79" s="65"/>
-      <c r="N79" s="69"/>
+      <c r="A79" s="97"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="67"/>
+      <c r="M79" s="66"/>
+      <c r="N79" s="70"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="96"/>
-      <c r="J80" s="65"/>
-      <c r="K80" s="66"/>
-      <c r="M80" s="65"/>
-      <c r="N80" s="69"/>
+      <c r="A80" s="97"/>
+      <c r="J80" s="66"/>
+      <c r="K80" s="67"/>
+      <c r="M80" s="66"/>
+      <c r="N80" s="70"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="96"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="69"/>
-      <c r="M81" s="65"/>
-      <c r="N81" s="69"/>
+      <c r="A81" s="97"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="70"/>
+      <c r="M81" s="66"/>
+      <c r="N81" s="70"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="96"/>
-      <c r="J82" s="100"/>
-      <c r="K82" s="77"/>
-      <c r="M82" s="65"/>
-      <c r="N82" s="69"/>
+      <c r="A82" s="97"/>
+      <c r="J82" s="101"/>
+      <c r="K82" s="78"/>
+      <c r="M82" s="66"/>
+      <c r="N82" s="70"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="96"/>
-      <c r="J83" s="76"/>
-      <c r="K83" s="77"/>
-      <c r="M83" s="71"/>
-      <c r="N83" s="83"/>
+      <c r="A83" s="97"/>
+      <c r="J83" s="77"/>
+      <c r="K83" s="78"/>
+      <c r="M83" s="72"/>
+      <c r="N83" s="84"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="96"/>
-      <c r="J84" s="76"/>
-      <c r="K84" s="101"/>
-      <c r="M84" s="102"/>
-      <c r="N84" s="66"/>
+      <c r="A84" s="97"/>
+      <c r="J84" s="77"/>
+      <c r="K84" s="102"/>
+      <c r="M84" s="103"/>
+      <c r="N84" s="67"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="96"/>
-      <c r="J85" s="76"/>
-      <c r="K85" s="77"/>
-      <c r="M85" s="103"/>
-      <c r="N85" s="66"/>
+      <c r="A85" s="97"/>
+      <c r="J85" s="77"/>
+      <c r="K85" s="78"/>
+      <c r="M85" s="104"/>
+      <c r="N85" s="67"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="96"/>
-      <c r="J86" s="76"/>
-      <c r="K86" s="77"/>
-      <c r="M86" s="103"/>
-      <c r="N86" s="66"/>
+      <c r="A86" s="97"/>
+      <c r="J86" s="77"/>
+      <c r="K86" s="78"/>
+      <c r="M86" s="104"/>
+      <c r="N86" s="67"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="96"/>
-      <c r="J87" s="76"/>
-      <c r="K87" s="86"/>
-      <c r="M87" s="104"/>
-      <c r="N87" s="66"/>
+      <c r="A87" s="97"/>
+      <c r="J87" s="77"/>
+      <c r="K87" s="87"/>
+      <c r="M87" s="105"/>
+      <c r="N87" s="67"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="96"/>
-      <c r="J88" s="85"/>
-      <c r="K88" s="75"/>
-      <c r="M88" s="71"/>
-      <c r="N88" s="69"/>
+      <c r="A88" s="97"/>
+      <c r="J88" s="86"/>
+      <c r="K88" s="76"/>
+      <c r="M88" s="72"/>
+      <c r="N88" s="70"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="96"/>
-      <c r="J89" s="81"/>
-      <c r="K89" s="75"/>
-      <c r="M89" s="65"/>
-      <c r="N89" s="69"/>
+      <c r="A89" s="97"/>
+      <c r="J89" s="82"/>
+      <c r="K89" s="76"/>
+      <c r="M89" s="66"/>
+      <c r="N89" s="70"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="96"/>
-      <c r="J90" s="81"/>
-      <c r="K90" s="75"/>
-      <c r="M90" s="65"/>
-      <c r="N90" s="66"/>
+      <c r="A90" s="97"/>
+      <c r="J90" s="82"/>
+      <c r="K90" s="76"/>
+      <c r="M90" s="66"/>
+      <c r="N90" s="67"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="96"/>
-      <c r="J91" s="88"/>
-      <c r="K91" s="98"/>
-      <c r="M91" s="65"/>
-      <c r="N91" s="66"/>
+      <c r="A91" s="97"/>
+      <c r="J91" s="89"/>
+      <c r="K91" s="99"/>
+      <c r="M91" s="66"/>
+      <c r="N91" s="67"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="96"/>
-      <c r="M92" s="71"/>
-      <c r="N92" s="69"/>
+      <c r="A92" s="97"/>
+      <c r="M92" s="72"/>
+      <c r="N92" s="70"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="96"/>
+      <c r="A93" s="97"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="96"/>
-      <c r="J94" s="35"/>
-      <c r="M94" s="71"/>
-      <c r="N94" s="83"/>
+      <c r="A94" s="97"/>
+      <c r="J94" s="36"/>
+      <c r="M94" s="72"/>
+      <c r="N94" s="84"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="96"/>
-      <c r="J95" s="65"/>
-      <c r="K95" s="66"/>
-      <c r="M95" s="103"/>
-      <c r="N95" s="66"/>
+      <c r="A95" s="97"/>
+      <c r="J95" s="66"/>
+      <c r="K95" s="67"/>
+      <c r="M95" s="104"/>
+      <c r="N95" s="67"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="96"/>
-      <c r="J96" s="65"/>
-      <c r="K96" s="66"/>
-      <c r="M96" s="71"/>
-      <c r="N96" s="69"/>
+      <c r="A96" s="97"/>
+      <c r="J96" s="66"/>
+      <c r="K96" s="67"/>
+      <c r="M96" s="72"/>
+      <c r="N96" s="70"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="96"/>
-      <c r="J97" s="65"/>
-      <c r="K97" s="66"/>
-      <c r="M97" s="103"/>
-      <c r="N97" s="105"/>
+      <c r="A97" s="97"/>
+      <c r="J97" s="66"/>
+      <c r="K97" s="67"/>
+      <c r="M97" s="104"/>
+      <c r="N97" s="106"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="96"/>
-      <c r="J98" s="65"/>
-      <c r="K98" s="69"/>
+      <c r="A98" s="97"/>
+      <c r="J98" s="66"/>
+      <c r="K98" s="70"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="96"/>
-      <c r="J99" s="74"/>
-      <c r="K99" s="75"/>
+      <c r="A99" s="97"/>
+      <c r="J99" s="75"/>
+      <c r="K99" s="76"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="96"/>
-      <c r="J100" s="76"/>
-      <c r="K100" s="77"/>
+      <c r="A100" s="97"/>
+      <c r="J100" s="77"/>
+      <c r="K100" s="78"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="96"/>
-      <c r="J101" s="71"/>
-      <c r="K101" s="69"/>
+      <c r="A101" s="97"/>
+      <c r="J101" s="72"/>
+      <c r="K101" s="70"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="96"/>
+      <c r="A102" s="97"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="96"/>
-      <c r="J103" s="35"/>
+      <c r="A103" s="97"/>
+      <c r="J103" s="36"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="96"/>
-      <c r="J104" s="65"/>
-      <c r="K104" s="66"/>
+      <c r="A104" s="97"/>
+      <c r="J104" s="66"/>
+      <c r="K104" s="67"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="96"/>
-      <c r="J105" s="65"/>
-      <c r="K105" s="66"/>
+      <c r="A105" s="97"/>
+      <c r="J105" s="66"/>
+      <c r="K105" s="67"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="96"/>
-      <c r="J106" s="65"/>
-      <c r="K106" s="69"/>
+      <c r="A106" s="97"/>
+      <c r="J106" s="66"/>
+      <c r="K106" s="70"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="96"/>
-      <c r="J107" s="65"/>
-      <c r="K107" s="66"/>
+      <c r="A107" s="97"/>
+      <c r="J107" s="66"/>
+      <c r="K107" s="67"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="96"/>
-      <c r="J108" s="74"/>
-      <c r="K108" s="75"/>
+      <c r="A108" s="97"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="76"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="96"/>
-      <c r="J109" s="76"/>
-      <c r="K109" s="77"/>
+      <c r="A109" s="97"/>
+      <c r="J109" s="77"/>
+      <c r="K109" s="78"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="96"/>
-      <c r="J110" s="71"/>
-      <c r="K110" s="69"/>
+      <c r="A110" s="97"/>
+      <c r="J110" s="72"/>
+      <c r="K110" s="70"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="96"/>
+      <c r="A111" s="97"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="96"/>
+      <c r="A112" s="97"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="96"/>
+      <c r="A113" s="97"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="96"/>
+      <c r="A114" s="97"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="96"/>
+      <c r="A115" s="97"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="96"/>
+      <c r="A116" s="97"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="96"/>
+      <c r="A117" s="97"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="96"/>
+      <c r="A118" s="97"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="96"/>
+      <c r="A119" s="97"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="96"/>
+      <c r="A120" s="97"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="96"/>
+      <c r="A121" s="97"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="96"/>
+      <c r="A122" s="97"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -2401,7 +2404,7 @@
       <c r="H122" s="4"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="96"/>
+      <c r="A123" s="97"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
@@ -2411,7 +2414,7 @@
       <c r="H123" s="4"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="96"/>
+      <c r="A124" s="97"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -2421,7 +2424,7 @@
       <c r="H124" s="4"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="96"/>
+      <c r="A125" s="97"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -2431,7 +2434,7 @@
       <c r="H125" s="4"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="96"/>
+      <c r="A126" s="97"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -2441,7 +2444,7 @@
       <c r="H126" s="4"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="96"/>
+      <c r="A127" s="97"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -2451,7 +2454,7 @@
       <c r="H127" s="4"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="96"/>
+      <c r="A128" s="97"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -2461,7 +2464,7 @@
       <c r="H128" s="4"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="96"/>
+      <c r="A129" s="97"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -2471,7 +2474,7 @@
       <c r="H129" s="4"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="96"/>
+      <c r="A130" s="97"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
@@ -2481,7 +2484,7 @@
       <c r="H130" s="4"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="96"/>
+      <c r="A131" s="97"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -2491,7 +2494,7 @@
       <c r="H131" s="4"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="96"/>
+      <c r="A132" s="97"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -7498,6 +7501,41 @@
   </sheetData>
   <autoFilter ref="$C$26:$D$60"/>
   <mergeCells count="69">
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="M66:N66"/>
     <mergeCell ref="G4:G8"/>
     <mergeCell ref="H4:H8"/>
     <mergeCell ref="B5:D5"/>
@@ -7521,52 +7559,17 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A24:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G62:H62"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.0" footer="0.0" header="0.0" left="0.18693402328589911" right="0.08796895213454076" top="0.2935435435435435"/>

</xml_diff>